<commit_message>
moved local logs to repo
</commit_message>
<xml_diff>
--- a/Course_Requirements/Activity Logs&Task Summaries/Jesse/ActivityLogSheetWk2.xlsx
+++ b/Course_Requirements/Activity Logs&Task Summaries/Jesse/ActivityLogSheetWk2.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="J:\uni\2019\S2-FINAL!!\CSC3600-ICT Professional Project\A3Stuff\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Jesse\Documents\GitHub\CSC3600-ICT-Professional-Project\Course_Requirements\Activity Logs&amp;Task Summaries\Jesse\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD8812DD-970C-4745-8938-E67A5A28F4B4}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C4587313-0DB4-45B0-92E2-EF3321289185}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="31125" yWindow="1695" windowWidth="21600" windowHeight="11385" xr2:uid="{9364D300-695B-4D0F-84F3-810C32CAA16B}"/>
+    <workbookView xWindow="28860" yWindow="30" windowWidth="13515" windowHeight="10125" xr2:uid="{9364D300-695B-4D0F-84F3-810C32CAA16B}"/>
   </bookViews>
   <sheets>
     <sheet name="ACTIVITY LOG SHEET " sheetId="2" r:id="rId1"/>
@@ -31,7 +31,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="16">
   <si>
     <t xml:space="preserve">ACTIVITY LOG SHEET </t>
   </si>
@@ -67,6 +67,18 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>Jesse Hare</t>
+  </si>
+  <si>
+    <t>Work on product specification</t>
+  </si>
+  <si>
+    <t>I</t>
+  </si>
+  <si>
+    <t>Work on project plan</t>
   </si>
 </sst>
 </file>
@@ -96,12 +108,14 @@
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
     <font>
       <i/>
       <sz val="12"/>
       <color theme="1"/>
       <name val="Cambria"/>
+      <family val="1"/>
     </font>
   </fonts>
   <fills count="2">
@@ -112,7 +126,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="19">
+  <borders count="17">
     <border>
       <left/>
       <right/>
@@ -224,32 +238,6 @@
         <color auto="1"/>
       </right>
       <top/>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left style="double">
-        <color auto="1"/>
-      </left>
-      <right/>
-      <top style="double">
-        <color auto="1"/>
-      </top>
-      <bottom style="dotted">
-        <color auto="1"/>
-      </bottom>
-      <diagonal/>
-    </border>
-    <border>
-      <left/>
-      <right style="double">
-        <color auto="1"/>
-      </right>
-      <top style="double">
-        <color auto="1"/>
-      </top>
       <bottom style="dotted">
         <color auto="1"/>
       </bottom>
@@ -357,7 +345,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="32">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="5" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
@@ -380,51 +368,46 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="16" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="17" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="18" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="14" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="14" fontId="3" fillId="0" borderId="15" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="14" fontId="3" fillId="0" borderId="16" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="17" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="9" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="8" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="7" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="164" fontId="3" fillId="0" borderId="6" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="14" fontId="3" fillId="0" borderId="18" xfId="1" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="13" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="14" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="15" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
@@ -434,28 +417,27 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -771,48 +753,58 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E7427381-DAAE-4995-9F49-4393536507A4}">
-  <dimension ref="A1:K25"/>
+  <dimension ref="A1:K24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E21" sqref="E21"/>
+      <selection activeCell="H9" sqref="H9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="16384" width="12.5703125" style="33"/>
+    <col min="1" max="1" width="12.5703125" style="19"/>
+    <col min="2" max="2" width="25.28515625" style="19" customWidth="1"/>
+    <col min="3" max="3" width="12.5703125" style="19"/>
+    <col min="4" max="4" width="13" style="19" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="12.5703125" style="19"/>
+    <col min="6" max="6" width="13.7109375" style="19" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="12.5703125" style="19"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A1" s="26" t="s">
+      <c r="A1" s="27" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="27"/>
-      <c r="C1" s="27"/>
-      <c r="D1" s="27"/>
-      <c r="E1" s="27"/>
-      <c r="F1" s="27"/>
-      <c r="G1" s="27"/>
-      <c r="H1" s="28"/>
+      <c r="B1" s="28"/>
+      <c r="C1" s="28"/>
+      <c r="D1" s="28"/>
+      <c r="E1" s="28"/>
+      <c r="F1" s="28"/>
+      <c r="G1" s="28"/>
+      <c r="H1" s="29"/>
     </row>
     <row r="2" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="29"/>
-      <c r="C2" s="27"/>
-      <c r="D2" s="27"/>
-      <c r="E2" s="28"/>
+      <c r="B2" s="30" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="28"/>
+      <c r="D2" s="28"/>
+      <c r="E2" s="29"/>
       <c r="F2" s="11" t="s">
         <v>2</v>
       </c>
-      <c r="G2" s="29"/>
-      <c r="H2" s="32"/>
+      <c r="G2" s="30">
+        <v>2</v>
+      </c>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A3" s="26" t="s">
+      <c r="A3" s="27" t="s">
         <v>3</v>
       </c>
-      <c r="B3" s="28"/>
+      <c r="B3" s="29"/>
       <c r="C3" s="3" t="s">
         <v>4</v>
       </c>
@@ -832,59 +824,119 @@
         <v>9</v>
       </c>
     </row>
-    <row r="4" spans="1:8" ht="16.5" thickTop="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="30"/>
-      <c r="B4" s="31"/>
-      <c r="C4" s="8"/>
-      <c r="D4" s="12"/>
-      <c r="E4" s="14"/>
-      <c r="F4" s="15"/>
+    <row r="4" spans="1:8" ht="16.5" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A4" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="26"/>
+      <c r="C4" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D4" s="12">
+        <v>43689</v>
+      </c>
+      <c r="E4" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="F4" s="15">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G4" s="5"/>
-      <c r="H4" s="6"/>
+      <c r="H4" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A5" s="19"/>
-      <c r="B5" s="20"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="14"/>
-      <c r="F5" s="15"/>
+      <c r="A5" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="26"/>
+      <c r="C5" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D5" s="13">
+        <v>43690</v>
+      </c>
+      <c r="E5" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="F5" s="15">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G5" s="5"/>
-      <c r="H5" s="6"/>
+      <c r="H5" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" s="19"/>
-      <c r="B6" s="20"/>
-      <c r="C6" s="9"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="14"/>
-      <c r="F6" s="15"/>
+      <c r="A6" s="25" t="s">
+        <v>15</v>
+      </c>
+      <c r="B6" s="26"/>
+      <c r="C6" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D6" s="13">
+        <v>43691</v>
+      </c>
+      <c r="E6" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="F6" s="15">
+        <v>0.5</v>
+      </c>
       <c r="G6" s="5"/>
-      <c r="H6" s="6"/>
+      <c r="H6" s="6">
+        <v>3</v>
+      </c>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" s="19"/>
-      <c r="B7" s="20"/>
-      <c r="C7" s="9"/>
-      <c r="D7" s="13"/>
-      <c r="E7" s="14"/>
-      <c r="F7" s="15"/>
+      <c r="A7" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="26"/>
+      <c r="C7" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" s="13">
+        <v>43692</v>
+      </c>
+      <c r="E7" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="F7" s="15">
+        <v>0.58333333333333337</v>
+      </c>
       <c r="G7" s="5"/>
-      <c r="H7" s="6"/>
+      <c r="H7" s="6">
+        <v>5</v>
+      </c>
     </row>
     <row r="8" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A8" s="19"/>
-      <c r="B8" s="20"/>
-      <c r="C8" s="9"/>
-      <c r="D8" s="13"/>
-      <c r="E8" s="14"/>
-      <c r="F8" s="15"/>
+      <c r="A8" s="25" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="26"/>
+      <c r="C8" s="9" t="s">
+        <v>14</v>
+      </c>
+      <c r="D8" s="13">
+        <v>43693</v>
+      </c>
+      <c r="E8" s="14">
+        <v>0.375</v>
+      </c>
+      <c r="F8" s="15">
+        <v>0.45833333333333331</v>
+      </c>
       <c r="G8" s="5"/>
-      <c r="H8" s="6"/>
+      <c r="H8" s="6">
+        <v>2</v>
+      </c>
     </row>
     <row r="9" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A9" s="19"/>
-      <c r="B9" s="20"/>
+      <c r="A9" s="25"/>
+      <c r="B9" s="26"/>
       <c r="C9" s="9"/>
       <c r="D9" s="13"/>
       <c r="E9" s="14"/>
@@ -893,8 +945,8 @@
       <c r="H9" s="6"/>
     </row>
     <row r="10" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A10" s="19"/>
-      <c r="B10" s="20"/>
+      <c r="A10" s="25"/>
+      <c r="B10" s="26"/>
       <c r="C10" s="9"/>
       <c r="D10" s="13"/>
       <c r="E10" s="14"/>
@@ -903,8 +955,8 @@
       <c r="H10" s="6"/>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A11" s="19"/>
-      <c r="B11" s="20"/>
+      <c r="A11" s="25"/>
+      <c r="B11" s="26"/>
       <c r="C11" s="9"/>
       <c r="D11" s="13"/>
       <c r="E11" s="14"/>
@@ -913,8 +965,8 @@
       <c r="H11" s="6"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A12" s="19"/>
-      <c r="B12" s="20"/>
+      <c r="A12" s="25"/>
+      <c r="B12" s="26"/>
       <c r="C12" s="9"/>
       <c r="D12" s="13"/>
       <c r="E12" s="14"/>
@@ -923,8 +975,8 @@
       <c r="H12" s="6"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A13" s="19"/>
-      <c r="B13" s="20"/>
+      <c r="A13" s="25"/>
+      <c r="B13" s="26"/>
       <c r="C13" s="9"/>
       <c r="D13" s="13"/>
       <c r="E13" s="14"/>
@@ -933,8 +985,8 @@
       <c r="H13" s="6"/>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A14" s="19"/>
-      <c r="B14" s="20"/>
+      <c r="A14" s="25"/>
+      <c r="B14" s="26"/>
       <c r="C14" s="9"/>
       <c r="D14" s="13"/>
       <c r="E14" s="14"/>
@@ -942,70 +994,59 @@
       <c r="G14" s="5"/>
       <c r="H14" s="6"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A15" s="19"/>
-      <c r="B15" s="20"/>
-      <c r="C15" s="9"/>
-      <c r="D15" s="13"/>
-      <c r="E15" s="14"/>
-      <c r="F15" s="15"/>
-      <c r="G15" s="5"/>
-      <c r="H15" s="6"/>
-    </row>
-    <row r="16" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A16" s="21"/>
-      <c r="B16" s="22"/>
-      <c r="C16" s="10"/>
-      <c r="D16" s="18"/>
-      <c r="E16" s="16"/>
-      <c r="F16" s="17"/>
-      <c r="G16" s="7"/>
-      <c r="H16" s="2"/>
-    </row>
-    <row r="17" spans="1:11" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A17" s="23" t="s">
+    <row r="15" spans="1:8" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="20"/>
+      <c r="B15" s="21"/>
+      <c r="C15" s="10"/>
+      <c r="D15" s="18"/>
+      <c r="E15" s="16"/>
+      <c r="F15" s="17"/>
+      <c r="G15" s="7"/>
+      <c r="H15" s="2"/>
+    </row>
+    <row r="16" spans="1:8" ht="17.25" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A16" s="22" t="s">
         <v>10</v>
       </c>
-      <c r="B17" s="24"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="24"/>
-      <c r="F17" s="25"/>
-      <c r="G17" s="2">
-        <f>SUM(G4:G16)</f>
+      <c r="B16" s="23"/>
+      <c r="C16" s="23"/>
+      <c r="D16" s="23"/>
+      <c r="E16" s="23"/>
+      <c r="F16" s="24"/>
+      <c r="G16" s="2">
+        <f>SUM(G4:G15)</f>
         <v>0</v>
       </c>
-      <c r="H17" s="2">
-        <f>SUM(H4:H16)</f>
-        <v>0</v>
-      </c>
-    </row>
-    <row r="18" spans="1:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
-      <c r="K25" s="33" t="s">
+      <c r="H16" s="2">
+        <f>SUM(H4:H15)</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="17" spans="11:11" ht="16.5" thickTop="1" x14ac:dyDescent="0.25"/>
+    <row r="24" spans="11:11" x14ac:dyDescent="0.25">
+      <c r="K24" s="19" t="s">
         <v>11</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="18">
-    <mergeCell ref="A16:B16"/>
-    <mergeCell ref="A17:F17"/>
-    <mergeCell ref="A8:B8"/>
-    <mergeCell ref="A9:B9"/>
-    <mergeCell ref="A10:B10"/>
-    <mergeCell ref="A13:B13"/>
-    <mergeCell ref="A14:B14"/>
-    <mergeCell ref="A15:B15"/>
-    <mergeCell ref="A11:B11"/>
-    <mergeCell ref="A12:B12"/>
+  <mergeCells count="17">
+    <mergeCell ref="A6:B6"/>
+    <mergeCell ref="G2:H2"/>
+    <mergeCell ref="A7:B7"/>
     <mergeCell ref="A1:H1"/>
     <mergeCell ref="B2:E2"/>
     <mergeCell ref="A3:B3"/>
     <mergeCell ref="A4:B4"/>
     <mergeCell ref="A5:B5"/>
-    <mergeCell ref="A6:B6"/>
-    <mergeCell ref="G2:H2"/>
-    <mergeCell ref="A7:B7"/>
+    <mergeCell ref="A15:B15"/>
+    <mergeCell ref="A16:F16"/>
+    <mergeCell ref="A8:B8"/>
+    <mergeCell ref="A9:B9"/>
+    <mergeCell ref="A12:B12"/>
+    <mergeCell ref="A13:B13"/>
+    <mergeCell ref="A14:B14"/>
+    <mergeCell ref="A10:B10"/>
+    <mergeCell ref="A11:B11"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="4294967292" verticalDpi="4294967292"/>

</xml_diff>